<commit_message>
chore: Clean up duplicate files and update component styles
</commit_message>
<xml_diff>
--- a/public/psych_pedia_drugs.xlsx
+++ b/public/psych_pedia_drugs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="741">
   <si>
     <t>ID</t>
   </si>
@@ -954,6 +954,12 @@
   </si>
   <si>
     <t>降低癫痫阈值，剂量大于450mg/d时风险显著。禁用于癫痫患者及进食障碍（贪食/厌食）患者。</t>
+  </si>
+  <si>
+    <t>双相抑郁治疗</t>
+  </si>
+  <si>
+    <t>可用于BD抑郁相治疗。转躁风险小。转躁风险依次为 安非他酮＜SSRIs＜SNRIs&lt;三环类</t>
   </si>
   <si>
     <t>mirtazapine</t>
@@ -3232,8 +3238,8 @@
   <sheetPr/>
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="13.5"/>
@@ -4674,48 +4680,48 @@
         <v>308</v>
       </c>
       <c r="X18" t="s">
-        <v>49</v>
+        <v>309</v>
       </c>
       <c r="Y18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="Z18" t="s">
-        <v>49</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:26">
       <c r="A19" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B19" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C19" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D19" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="E19" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F19" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="G19" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="H19" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="I19" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="J19" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="K19" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="L19" t="s">
         <v>79</v>
@@ -4727,31 +4733,31 @@
         <v>39</v>
       </c>
       <c r="O19" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="P19" t="s">
         <v>47</v>
       </c>
       <c r="Q19" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="R19" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="S19" t="s">
         <v>47</v>
       </c>
       <c r="T19" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="U19" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="V19" t="s">
         <v>44</v>
       </c>
       <c r="W19" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="X19" t="s">
         <v>49</v>
@@ -4765,22 +4771,22 @@
     </row>
     <row r="20" spans="1:26">
       <c r="A20" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B20" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C20" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D20" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E20" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F20" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G20" t="s">
         <v>220</v>
@@ -4789,13 +4795,13 @@
         <v>189</v>
       </c>
       <c r="I20" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="J20" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="K20" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="L20" t="s">
         <v>113</v>
@@ -4807,31 +4813,31 @@
         <v>39</v>
       </c>
       <c r="O20" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="P20" t="s">
         <v>47</v>
       </c>
       <c r="Q20" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="R20" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="S20" t="s">
         <v>44</v>
       </c>
       <c r="T20" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="U20" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="V20" t="s">
         <v>67</v>
       </c>
       <c r="W20" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="X20" t="s">
         <v>49</v>
@@ -4845,37 +4851,37 @@
     </row>
     <row r="21" spans="1:26">
       <c r="A21" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B21" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C21" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D21" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E21" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F21" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="G21" t="s">
         <v>171</v>
       </c>
       <c r="H21" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="I21" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="J21" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="K21" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="L21" t="s">
         <v>113</v>
@@ -4887,31 +4893,31 @@
         <v>39</v>
       </c>
       <c r="O21" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="P21" t="s">
         <v>44</v>
       </c>
       <c r="Q21" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="R21" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="S21" t="s">
         <v>41</v>
       </c>
       <c r="T21" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="U21" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="V21" t="s">
         <v>47</v>
       </c>
       <c r="W21" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="X21" t="s">
         <v>49</v>
@@ -4925,73 +4931,73 @@
     </row>
     <row r="22" spans="1:26">
       <c r="A22" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B22" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C22" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D22" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E22" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="F22" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="G22" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="H22" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="I22" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="J22" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="K22" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="L22" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="M22" t="s">
         <v>38</v>
       </c>
       <c r="N22" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="O22" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="P22" t="s">
         <v>47</v>
       </c>
       <c r="Q22" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="R22" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="S22" t="s">
         <v>41</v>
       </c>
       <c r="T22" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="U22" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="V22" t="s">
         <v>67</v>
       </c>
       <c r="W22" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="X22" t="s">
         <v>49</v>
@@ -5005,37 +5011,37 @@
     </row>
     <row r="23" spans="1:26">
       <c r="A23" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B23" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C23" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D23" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E23" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="F23" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="G23" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="H23" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="I23" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="J23" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="K23" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="L23" t="s">
         <v>79</v>
@@ -5044,34 +5050,34 @@
         <v>38</v>
       </c>
       <c r="N23" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="O23" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="P23" t="s">
         <v>47</v>
       </c>
       <c r="Q23" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="R23" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="S23" t="s">
         <v>41</v>
       </c>
       <c r="T23" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="U23" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="V23" t="s">
         <v>67</v>
       </c>
       <c r="W23" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="X23" t="s">
         <v>49</v>
@@ -5085,37 +5091,37 @@
     </row>
     <row r="24" spans="1:26">
       <c r="A24" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B24" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C24" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D24" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E24" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F24" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="G24" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="H24" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="I24" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="J24" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="K24" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="L24" t="s">
         <v>95</v>
@@ -5127,31 +5133,31 @@
         <v>39</v>
       </c>
       <c r="O24" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="P24" t="s">
         <v>47</v>
       </c>
       <c r="Q24" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="R24" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="S24" t="s">
         <v>41</v>
       </c>
       <c r="T24" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="U24" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="V24" t="s">
         <v>67</v>
       </c>
       <c r="W24" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="X24" t="s">
         <v>49</v>
@@ -5165,22 +5171,22 @@
     </row>
     <row r="25" spans="1:26">
       <c r="A25" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B25" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C25" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="D25" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E25" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="F25" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="G25" t="s">
         <v>253</v>
@@ -5189,13 +5195,13 @@
         <v>109</v>
       </c>
       <c r="I25" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="J25" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="K25" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="L25" t="s">
         <v>79</v>
@@ -5207,31 +5213,31 @@
         <v>239</v>
       </c>
       <c r="O25" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="P25" t="s">
         <v>47</v>
       </c>
       <c r="Q25" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="R25" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="S25" t="s">
         <v>41</v>
       </c>
       <c r="T25" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="U25" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="V25" t="s">
         <v>44</v>
       </c>
       <c r="W25" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="X25" t="s">
         <v>49</v>
@@ -5245,37 +5251,37 @@
     </row>
     <row r="26" spans="1:26">
       <c r="A26" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B26" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C26" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D26" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E26" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="F26" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="G26" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="H26" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="I26" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="J26" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="K26" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="L26" t="s">
         <v>79</v>
@@ -5287,31 +5293,31 @@
         <v>239</v>
       </c>
       <c r="O26" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="P26" t="s">
         <v>47</v>
       </c>
       <c r="Q26" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="R26" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="S26" t="s">
         <v>44</v>
       </c>
       <c r="T26" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="U26" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="V26" t="s">
         <v>67</v>
       </c>
       <c r="W26" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="X26" t="s">
         <v>49</v>
@@ -5325,37 +5331,37 @@
     </row>
     <row r="27" spans="1:26">
       <c r="A27" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B27" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C27" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D27" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="E27" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="F27" t="s">
         <v>173</v>
       </c>
       <c r="G27" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="H27" t="s">
         <v>109</v>
       </c>
       <c r="I27" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="J27" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="K27" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="L27" t="s">
         <v>95</v>
@@ -5367,31 +5373,31 @@
         <v>39</v>
       </c>
       <c r="O27" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="P27" t="s">
         <v>47</v>
       </c>
       <c r="Q27" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="R27" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="S27" t="s">
         <v>41</v>
       </c>
       <c r="T27" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="U27" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="V27" t="s">
         <v>67</v>
       </c>
       <c r="W27" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="X27" t="s">
         <v>49</v>
@@ -5405,37 +5411,37 @@
     </row>
     <row r="28" spans="1:26">
       <c r="A28" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B28" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C28" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D28" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="E28" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="F28" t="s">
         <v>57</v>
       </c>
       <c r="G28" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="H28" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="I28" t="s">
         <v>76</v>
       </c>
       <c r="J28" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="K28" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="L28" t="s">
         <v>95</v>
@@ -5447,31 +5453,31 @@
         <v>39</v>
       </c>
       <c r="O28" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="P28" t="s">
         <v>47</v>
       </c>
       <c r="Q28" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="R28" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="S28" t="s">
         <v>67</v>
       </c>
       <c r="T28" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="U28" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="V28" t="s">
         <v>44</v>
       </c>
       <c r="W28" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="X28" t="s">
         <v>49</v>
@@ -5485,37 +5491,37 @@
     </row>
     <row r="29" spans="1:26">
       <c r="A29" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B29" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C29" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D29" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E29" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="F29" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="G29" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="H29" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="I29" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="J29" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="K29" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="L29" t="s">
         <v>113</v>
@@ -5527,31 +5533,31 @@
         <v>39</v>
       </c>
       <c r="O29" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="P29" t="s">
         <v>47</v>
       </c>
       <c r="Q29" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="R29" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="S29" t="s">
         <v>44</v>
       </c>
       <c r="T29" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="U29" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="V29" t="s">
         <v>67</v>
       </c>
       <c r="W29" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="X29" t="s">
         <v>49</v>
@@ -5565,22 +5571,22 @@
     </row>
     <row r="30" spans="1:26">
       <c r="A30" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B30" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C30" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D30" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E30" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="F30" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="G30" t="s">
         <v>220</v>
@@ -5589,13 +5595,13 @@
         <v>189</v>
       </c>
       <c r="I30" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="J30" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="K30" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="L30" t="s">
         <v>95</v>
@@ -5607,31 +5613,31 @@
         <v>39</v>
       </c>
       <c r="O30" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="P30" t="s">
         <v>44</v>
       </c>
       <c r="Q30" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="R30" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="S30" t="s">
         <v>67</v>
       </c>
       <c r="T30" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="U30" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="V30" t="s">
         <v>41</v>
       </c>
       <c r="W30" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="X30" t="s">
         <v>49</v>
@@ -5645,37 +5651,37 @@
     </row>
     <row r="31" spans="1:26">
       <c r="A31" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B31" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C31" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D31" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="E31" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="F31" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="G31" t="s">
         <v>171</v>
       </c>
       <c r="H31" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="I31" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="J31" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="K31" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="L31" t="s">
         <v>79</v>
@@ -5684,34 +5690,34 @@
         <v>38</v>
       </c>
       <c r="N31" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="O31" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="P31" t="s">
         <v>47</v>
       </c>
       <c r="Q31" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="R31" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="S31" t="s">
         <v>44</v>
       </c>
       <c r="T31" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="U31" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="V31" t="s">
         <v>67</v>
       </c>
       <c r="W31" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="X31" t="s">
         <v>49</v>
@@ -5725,25 +5731,25 @@
     </row>
     <row r="32" spans="1:26">
       <c r="A32" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B32" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C32" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D32" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E32" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="F32" t="s">
         <v>57</v>
       </c>
       <c r="G32" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="H32" t="s">
         <v>150</v>
@@ -5752,10 +5758,10 @@
         <v>76</v>
       </c>
       <c r="J32" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="K32" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="L32" t="s">
         <v>95</v>
@@ -5767,31 +5773,31 @@
         <v>39</v>
       </c>
       <c r="O32" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="P32" t="s">
         <v>44</v>
       </c>
       <c r="Q32" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="R32" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="S32" t="s">
         <v>47</v>
       </c>
       <c r="T32" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="U32" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="V32" t="s">
         <v>41</v>
       </c>
       <c r="W32" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="X32" t="s">
         <v>49</v>
@@ -5805,37 +5811,37 @@
     </row>
     <row r="33" spans="1:26">
       <c r="A33" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B33" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="C33" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="D33" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E33" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="F33" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="G33" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="H33" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="I33" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="J33" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="K33" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="L33" t="s">
         <v>95</v>
@@ -5847,31 +5853,31 @@
         <v>39</v>
       </c>
       <c r="O33" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="P33" t="s">
         <v>47</v>
       </c>
       <c r="Q33" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="R33" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="S33" t="s">
         <v>41</v>
       </c>
       <c r="T33" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="U33" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="V33" t="s">
         <v>67</v>
       </c>
       <c r="W33" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="X33" t="s">
         <v>49</v>
@@ -5885,37 +5891,37 @@
     </row>
     <row r="34" spans="1:26">
       <c r="A34" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B34" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C34" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="D34" t="s">
         <v>186</v>
       </c>
       <c r="E34" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="F34" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="G34" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="H34" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="I34" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="J34" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="K34" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="L34" t="s">
         <v>79</v>
@@ -5927,31 +5933,31 @@
         <v>39</v>
       </c>
       <c r="O34" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="P34" t="s">
         <v>44</v>
       </c>
       <c r="Q34" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="R34" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="S34" t="s">
         <v>41</v>
       </c>
       <c r="T34" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="U34" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="V34" t="s">
         <v>67</v>
       </c>
       <c r="W34" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="X34" t="s">
         <v>49</v>
@@ -5965,37 +5971,37 @@
     </row>
     <row r="35" spans="1:26">
       <c r="A35" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="B35" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="C35" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="D35" t="s">
         <v>201</v>
       </c>
       <c r="E35" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="F35" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="G35" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="H35" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="I35" t="s">
         <v>127</v>
       </c>
       <c r="J35" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="K35" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="L35" t="s">
         <v>79</v>
@@ -6007,31 +6013,31 @@
         <v>39</v>
       </c>
       <c r="O35" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="P35" t="s">
         <v>47</v>
       </c>
       <c r="Q35" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="R35" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="S35" t="s">
         <v>44</v>
       </c>
       <c r="T35" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="U35" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="V35" t="s">
         <v>41</v>
       </c>
       <c r="W35" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="X35" t="s">
         <v>49</v>
@@ -6045,22 +6051,22 @@
     </row>
     <row r="36" spans="1:26">
       <c r="A36" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B36" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C36" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="D36" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="E36" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="F36" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="G36" t="s">
         <v>74</v>
@@ -6069,13 +6075,13 @@
         <v>109</v>
       </c>
       <c r="I36" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="J36" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="K36" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="L36" t="s">
         <v>79</v>
@@ -6087,31 +6093,31 @@
         <v>39</v>
       </c>
       <c r="O36" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="P36" t="s">
         <v>47</v>
       </c>
       <c r="Q36" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="R36" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="S36" t="s">
         <v>44</v>
       </c>
       <c r="T36" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="U36" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="V36" t="s">
         <v>41</v>
       </c>
       <c r="W36" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="X36" t="s">
         <v>49</v>
@@ -6125,37 +6131,37 @@
     </row>
     <row r="37" spans="1:26">
       <c r="A37" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B37" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C37" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="D37" t="s">
         <v>186</v>
       </c>
       <c r="E37" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="F37" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="G37" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="H37" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="I37" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="J37" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="K37" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="L37" t="s">
         <v>176</v>
@@ -6167,75 +6173,75 @@
         <v>39</v>
       </c>
       <c r="O37" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="P37" t="s">
         <v>44</v>
       </c>
       <c r="Q37" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="R37" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="S37" t="s">
         <v>67</v>
       </c>
       <c r="T37" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="U37" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="V37" t="s">
         <v>41</v>
       </c>
       <c r="W37" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="X37" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="Y37" t="s">
         <v>41</v>
       </c>
       <c r="Z37" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="38" spans="1:26">
       <c r="A38" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="B38" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="C38" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D38" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="E38" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="F38" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="G38" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="H38" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="I38" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="J38" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="K38" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="L38" t="s">
         <v>79</v>
@@ -6247,31 +6253,31 @@
         <v>39</v>
       </c>
       <c r="O38" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="P38" t="s">
         <v>47</v>
       </c>
       <c r="Q38" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="R38" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="S38" t="s">
         <v>41</v>
       </c>
       <c r="T38" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="U38" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="V38" t="s">
         <v>44</v>
       </c>
       <c r="W38" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="X38" t="s">
         <v>49</v>
@@ -6285,37 +6291,37 @@
     </row>
     <row r="39" spans="1:26">
       <c r="A39" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="B39" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="C39" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="D39" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E39" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="F39" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="G39" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="H39" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="I39" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="J39" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="K39" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="L39" t="s">
         <v>79</v>
@@ -6327,31 +6333,31 @@
         <v>239</v>
       </c>
       <c r="O39" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="P39" t="s">
         <v>44</v>
       </c>
       <c r="Q39" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="R39" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="S39" t="s">
         <v>41</v>
       </c>
       <c r="T39" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="U39" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="V39" t="s">
         <v>67</v>
       </c>
       <c r="W39" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="X39" t="s">
         <v>49</v>
@@ -6365,31 +6371,31 @@
     </row>
     <row r="40" spans="1:26">
       <c r="A40" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="B40" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="C40" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="D40" t="s">
         <v>186</v>
       </c>
       <c r="E40" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="F40" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="G40" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="H40" t="s">
         <v>92</v>
       </c>
       <c r="I40" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="J40" t="s">
         <v>144</v>
@@ -6407,31 +6413,31 @@
         <v>39</v>
       </c>
       <c r="O40" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="P40" t="s">
         <v>44</v>
       </c>
       <c r="Q40" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="R40" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="S40" t="s">
         <v>41</v>
       </c>
       <c r="T40" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="U40" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="V40" t="s">
         <v>47</v>
       </c>
       <c r="W40" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="X40" t="s">
         <v>49</v>
@@ -6445,37 +6451,37 @@
     </row>
     <row r="41" spans="1:26">
       <c r="A41" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="B41" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="C41" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="D41" t="s">
         <v>29</v>
       </c>
       <c r="E41" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="F41" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="G41" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="H41" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="I41" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="J41" t="s">
         <v>77</v>
       </c>
       <c r="K41" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="L41" t="s">
         <v>95</v>
@@ -6487,31 +6493,31 @@
         <v>39</v>
       </c>
       <c r="O41" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="P41" t="s">
         <v>41</v>
       </c>
       <c r="Q41" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="R41" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="S41" t="s">
         <v>47</v>
       </c>
       <c r="T41" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="U41" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="V41" t="s">
         <v>67</v>
       </c>
       <c r="W41" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="X41" t="s">
         <v>49</v>
@@ -6525,37 +6531,37 @@
     </row>
     <row r="42" spans="1:26">
       <c r="A42" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B42" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="C42" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="D42" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="E42" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="F42" t="s">
         <v>235</v>
       </c>
       <c r="G42" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="H42" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="I42" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="J42" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="K42" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="L42" t="s">
         <v>95</v>
@@ -6567,31 +6573,31 @@
         <v>239</v>
       </c>
       <c r="O42" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="P42" t="s">
         <v>47</v>
       </c>
       <c r="Q42" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="R42" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="S42" t="s">
         <v>41</v>
       </c>
       <c r="T42" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="U42" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="V42" t="s">
         <v>67</v>
       </c>
       <c r="W42" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="X42" t="s">
         <v>49</v>
@@ -6605,37 +6611,37 @@
     </row>
     <row r="43" spans="1:26">
       <c r="A43" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B43" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="C43" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="D43" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E43" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="F43" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="G43" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="H43" t="s">
         <v>109</v>
       </c>
       <c r="I43" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="J43" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="K43" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="L43" t="s">
         <v>79</v>
@@ -6647,31 +6653,31 @@
         <v>239</v>
       </c>
       <c r="O43" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="P43" t="s">
         <v>44</v>
       </c>
       <c r="Q43" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="R43" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="S43" t="s">
         <v>41</v>
       </c>
       <c r="T43" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="U43" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="V43" t="s">
         <v>67</v>
       </c>
       <c r="W43" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="X43" t="s">
         <v>49</v>
@@ -6685,37 +6691,37 @@
     </row>
     <row r="44" spans="1:26">
       <c r="A44" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B44" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="C44" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="D44" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="E44" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="F44" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="G44" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="H44" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="I44" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="J44" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="K44" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="L44" t="s">
         <v>79</v>
@@ -6727,31 +6733,31 @@
         <v>39</v>
       </c>
       <c r="O44" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="P44" t="s">
         <v>67</v>
       </c>
       <c r="Q44" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="R44" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="S44" t="s">
         <v>44</v>
       </c>
       <c r="T44" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="U44" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="V44" t="s">
         <v>41</v>
       </c>
       <c r="W44" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="X44" t="s">
         <v>49</v>
@@ -6765,37 +6771,37 @@
     </row>
     <row r="45" spans="1:26">
       <c r="A45" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B45" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C45" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="D45" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="E45" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="F45" t="s">
         <v>173</v>
       </c>
       <c r="G45" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="H45" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="I45" t="s">
         <v>76</v>
       </c>
       <c r="J45" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="K45" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="L45" t="s">
         <v>95</v>
@@ -6807,31 +6813,31 @@
         <v>39</v>
       </c>
       <c r="O45" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="P45" t="s">
         <v>44</v>
       </c>
       <c r="Q45" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="R45" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="S45" t="s">
         <v>41</v>
       </c>
       <c r="T45" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="U45" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="V45" t="s">
         <v>47</v>
       </c>
       <c r="W45" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="X45" t="s">
         <v>49</v>
@@ -6845,37 +6851,37 @@
     </row>
     <row r="46" spans="1:26">
       <c r="A46" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B46" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="C46" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="D46" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="E46" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="F46" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="G46" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="H46" t="s">
         <v>109</v>
       </c>
       <c r="I46" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="J46" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="K46" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="L46" t="s">
         <v>95</v>
@@ -6887,31 +6893,31 @@
         <v>39</v>
       </c>
       <c r="O46" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="P46" t="s">
         <v>44</v>
       </c>
       <c r="Q46" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="R46" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="S46" t="s">
         <v>47</v>
       </c>
       <c r="T46" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="U46" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="V46" t="s">
         <v>41</v>
       </c>
       <c r="W46" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="X46" t="s">
         <v>49</v>

</xml_diff>